<commit_message>
data save to different folder
</commit_message>
<xml_diff>
--- a/RoomID.xlsx
+++ b/RoomID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitWork\Airbnb data Analyst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EE9976-2203-4B71-B100-EEF9EEBAEB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE9CD79-587D-493C-8727-6A5C15095F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5760" windowWidth="22536" windowHeight="8280" xr2:uid="{D7A8E803-04FB-4918-B9B3-6FD0BB9BB951}"/>
+    <workbookView xWindow="1056" yWindow="2760" windowWidth="27492" windowHeight="12048" xr2:uid="{D7A8E803-04FB-4918-B9B3-6FD0BB9BB951}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>830193102361409290</t>
   </si>
@@ -48,6 +48,18 @@
   </si>
   <si>
     <t>43435162</t>
+  </si>
+  <si>
+    <t>837352260137971048</t>
+  </si>
+  <si>
+    <t>49525472</t>
+  </si>
+  <si>
+    <t>716883705085875481</t>
+  </si>
+  <si>
+    <t>969823904189469776</t>
   </si>
 </sst>
 </file>
@@ -83,15 +95,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -427,40 +440,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4266EB53-8B1B-4BB5-9A15-F5260CB5C087}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1">
         <v>3</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>